<commit_message>
Lancer G6 support cleanup. Prep for saving package data and payload verification.
</commit_message>
<xml_diff>
--- a/16A-Red-BOM-2015-12-10.xlsx
+++ b/16A-Red-BOM-2015-12-10.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26505"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bbothwell/Box Sync/UX Packages/UX Package BOMs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26423"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="-25600" yWindow="700" windowWidth="25600" windowHeight="17540"/>
   </bookViews>
@@ -571,9 +566,6 @@
     <t>BE3-R (NIC, iSCSI, FCoE)</t>
   </si>
   <si>
-    <t>Lancer (FC)</t>
-  </si>
-  <si>
     <t>Saturn (FC)</t>
   </si>
   <si>
@@ -1107,6 +1099,9 @@
   </si>
   <si>
     <t>Removed ESXi 5.1 support per Manzar</t>
+  </si>
+  <si>
+    <t>Lancer G5 (FC)</t>
   </si>
 </sst>
 </file>
@@ -1845,6 +1840,37 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1871,37 +1897,6 @@
     </xf>
     <xf numFmtId="16" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="230">
@@ -2189,7 +2184,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2224,7 +2219,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2436,10 +2431,10 @@
   <dimension ref="A1:P76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="H12" sqref="H12:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="2.1640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="24.6640625" style="2" customWidth="1"/>
@@ -2458,42 +2453,42 @@
     <col min="15" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="114" t="s">
-        <v>318</v>
-      </c>
-      <c r="B1" s="114"/>
+    <row r="1" spans="1:16" ht="18">
+      <c r="A1" s="111" t="s">
+        <v>317</v>
+      </c>
+      <c r="B1" s="111"/>
       <c r="C1" s="94"/>
       <c r="D1" s="94"/>
     </row>
-    <row r="2" spans="1:16" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="114" t="s">
-        <v>281</v>
-      </c>
-      <c r="B2" s="114"/>
-    </row>
-    <row r="4" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="18">
+      <c r="A2" s="111" t="s">
+        <v>280</v>
+      </c>
+      <c r="B2" s="111"/>
+    </row>
+    <row r="4" spans="1:16" ht="15">
       <c r="B4" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="113" t="s">
-        <v>283</v>
-      </c>
-      <c r="E4" s="113"/>
-      <c r="F4" s="113"/>
+      <c r="D4" s="110" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="113" t="s">
+      <c r="H4" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="113"/>
-      <c r="J4" s="113"/>
-      <c r="K4" s="113"/>
-      <c r="L4" s="113"/>
-      <c r="M4" s="113"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="110"/>
       <c r="N4" s="14"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="B5" s="75" t="s">
         <v>33</v>
       </c>
@@ -2524,36 +2519,36 @@
         <v>35</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N5" s="20"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="B6" s="76" t="s">
         <v>32</v>
       </c>
       <c r="C6" s="16"/>
-      <c r="D6" s="110" t="s">
+      <c r="D6" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="111"/>
-      <c r="F6" s="112"/>
+      <c r="E6" s="108"/>
+      <c r="F6" s="109"/>
       <c r="G6" s="21"/>
-      <c r="H6" s="110" t="s">
+      <c r="H6" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="112"/>
+      <c r="I6" s="108"/>
+      <c r="J6" s="108"/>
+      <c r="K6" s="108"/>
+      <c r="L6" s="108"/>
+      <c r="M6" s="109"/>
       <c r="N6" s="22"/>
       <c r="O6" s="68"/>
       <c r="P6" s="23"/>
     </row>
-    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="28">
       <c r="B7" s="77" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C7" s="24"/>
       <c r="D7" s="25" t="s">
@@ -2567,7 +2562,7 @@
       </c>
       <c r="G7" s="28"/>
       <c r="H7" s="84" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I7" s="82" t="s">
         <v>144</v>
@@ -2582,15 +2577,15 @@
         <v>41</v>
       </c>
       <c r="M7" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="N7" s="22"/>
       <c r="O7" s="68"/>
       <c r="P7" s="30"/>
     </row>
-    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="28">
       <c r="B8" s="77" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C8" s="24"/>
       <c r="D8" s="29" t="s">
@@ -2604,29 +2599,29 @@
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="84" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I8" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="J8" s="39" t="s">
         <v>205</v>
       </c>
-      <c r="J8" s="39" t="s">
+      <c r="K8" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="L8" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="L8" s="38" t="s">
-        <v>208</v>
-      </c>
       <c r="M8" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O8" s="68"/>
       <c r="P8" s="30"/>
     </row>
-    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="28">
       <c r="B9" s="79" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C9" s="24"/>
       <c r="D9" s="25" t="s">
@@ -2640,29 +2635,29 @@
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="95" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="I9" s="39" t="s">
+        <v>208</v>
+      </c>
+      <c r="J9" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="J9" s="39" t="s">
+      <c r="K9" s="39" t="s">
+        <v>209</v>
+      </c>
+      <c r="L9" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="K9" s="39" t="s">
-        <v>210</v>
-      </c>
-      <c r="L9" s="38" t="s">
-        <v>211</v>
-      </c>
       <c r="M9" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O9" s="68"/>
       <c r="P9" s="30"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="B10" s="77" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="15" t="s">
@@ -2678,9 +2673,9 @@
       <c r="O10" s="68"/>
       <c r="P10" s="30"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="B11" s="79" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="25" t="s">
@@ -2693,24 +2688,24 @@
         <v>5</v>
       </c>
       <c r="G11" s="37"/>
-      <c r="H11" s="118" t="s">
-        <v>171</v>
-      </c>
-      <c r="I11" s="118"/>
-      <c r="J11" s="118"/>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
+      <c r="H11" s="104" t="s">
+        <v>338</v>
+      </c>
+      <c r="I11" s="104"/>
+      <c r="J11" s="104"/>
+      <c r="K11" s="104"/>
+      <c r="L11" s="104"/>
+      <c r="M11" s="104"/>
       <c r="O11" s="68"/>
       <c r="P11" s="30"/>
     </row>
-    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="28">
       <c r="B12" s="77" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="25" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E12" s="35">
         <v>5467</v>
@@ -2719,8 +2714,8 @@
         <v>6</v>
       </c>
       <c r="G12" s="28"/>
-      <c r="H12" s="119" t="s">
-        <v>312</v>
+      <c r="H12" s="105" t="s">
+        <v>311</v>
       </c>
       <c r="I12" s="91" t="s">
         <v>153</v>
@@ -2735,18 +2730,18 @@
         <v>150</v>
       </c>
       <c r="M12" s="82" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O12" s="68"/>
       <c r="P12" s="30"/>
     </row>
-    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="28">
       <c r="B13" s="77" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="39" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E13" s="35">
         <v>8753</v>
@@ -2755,7 +2750,7 @@
         <v>7</v>
       </c>
       <c r="G13" s="28"/>
-      <c r="H13" s="120"/>
+      <c r="H13" s="106"/>
       <c r="I13" s="82" t="s">
         <v>155</v>
       </c>
@@ -2763,24 +2758,24 @@
         <v>151</v>
       </c>
       <c r="K13" s="82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L13" s="82" t="s">
         <v>152</v>
       </c>
       <c r="M13" s="82" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O13" s="68"/>
       <c r="P13" s="30"/>
     </row>
-    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="28">
       <c r="B14" s="77" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C14" s="40"/>
       <c r="D14" s="29" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E14" s="31">
         <v>8869</v>
@@ -2789,33 +2784,33 @@
         <v>8</v>
       </c>
       <c r="H14" s="100" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I14" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="J14" s="83" t="s">
+        <v>211</v>
+      </c>
+      <c r="K14" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="J14" s="83" t="s">
+      <c r="L14" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="K14" s="38" t="s">
-        <v>217</v>
-      </c>
-      <c r="L14" s="38" t="s">
-        <v>213</v>
-      </c>
       <c r="M14" s="82" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O14" s="68"/>
       <c r="P14" s="30"/>
     </row>
-    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="28">
       <c r="B15" s="79" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="25" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E15" s="35">
         <v>8871</v>
@@ -2824,36 +2819,36 @@
         <v>9</v>
       </c>
       <c r="H15" s="84" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I15" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="J15" s="39" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="L15" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="K15" s="38" t="s">
-        <v>219</v>
-      </c>
-      <c r="L15" s="38" t="s">
-        <v>215</v>
-      </c>
       <c r="M15" s="82" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="O15" s="68"/>
       <c r="P15" s="30"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="B16" s="79" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C16" s="40"/>
       <c r="D16" s="25" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F16" s="27">
         <v>10</v>
@@ -2861,101 +2856,101 @@
       <c r="O16" s="68"/>
       <c r="P16" s="30"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16">
       <c r="B17" s="78" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C17" s="44"/>
       <c r="D17" s="50"/>
       <c r="E17" s="97"/>
       <c r="F17" s="98"/>
       <c r="G17" s="68"/>
-      <c r="H17" s="118" t="s">
-        <v>334</v>
-      </c>
-      <c r="I17" s="118"/>
-      <c r="J17" s="118"/>
-      <c r="K17" s="118"/>
-      <c r="L17" s="118"/>
-      <c r="M17" s="118"/>
+      <c r="H17" s="104" t="s">
+        <v>333</v>
+      </c>
+      <c r="I17" s="104"/>
+      <c r="J17" s="104"/>
+      <c r="K17" s="104"/>
+      <c r="L17" s="104"/>
+      <c r="M17" s="104"/>
       <c r="O17" s="68"/>
       <c r="P17" s="30"/>
     </row>
-    <row r="18" spans="2:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="28">
       <c r="B18" s="77" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C18" s="8"/>
-      <c r="D18" s="115" t="s">
-        <v>204</v>
-      </c>
-      <c r="E18" s="116"/>
-      <c r="F18" s="117"/>
+      <c r="D18" s="101" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" s="102"/>
+      <c r="F18" s="103"/>
       <c r="G18" s="68"/>
-      <c r="H18" s="119" t="s">
-        <v>312</v>
+      <c r="H18" s="105" t="s">
+        <v>311</v>
       </c>
       <c r="I18" s="82" t="s">
+        <v>318</v>
+      </c>
+      <c r="J18" s="92" t="s">
+        <v>320</v>
+      </c>
+      <c r="K18" s="91" t="s">
         <v>319</v>
       </c>
-      <c r="J18" s="92" t="s">
+      <c r="L18" s="91" t="s">
         <v>321</v>
       </c>
-      <c r="K18" s="91" t="s">
-        <v>320</v>
-      </c>
-      <c r="L18" s="91" t="s">
-        <v>322</v>
-      </c>
       <c r="M18" s="82" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="O18" s="68"/>
       <c r="P18" s="30"/>
     </row>
-    <row r="19" spans="2:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" ht="28">
       <c r="B19" s="78" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="83" t="s">
+        <v>195</v>
+      </c>
+      <c r="E19" s="71" t="s">
         <v>196</v>
-      </c>
-      <c r="E19" s="71" t="s">
-        <v>197</v>
       </c>
       <c r="F19" s="42">
         <v>50</v>
       </c>
       <c r="G19" s="68"/>
-      <c r="H19" s="120"/>
+      <c r="H19" s="106"/>
       <c r="I19" s="82" t="s">
+        <v>322</v>
+      </c>
+      <c r="J19" s="83" t="s">
+        <v>324</v>
+      </c>
+      <c r="K19" s="82" t="s">
+        <v>325</v>
+      </c>
+      <c r="L19" s="82" t="s">
         <v>323</v>
       </c>
-      <c r="J19" s="83" t="s">
-        <v>325</v>
-      </c>
-      <c r="K19" s="82" t="s">
+      <c r="M19" s="82" t="s">
         <v>326</v>
       </c>
-      <c r="L19" s="82" t="s">
-        <v>324</v>
-      </c>
-      <c r="M19" s="82" t="s">
-        <v>327</v>
-      </c>
       <c r="O19" s="68"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16">
       <c r="B20" s="77" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="83" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" s="41" t="s">
         <v>198</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>199</v>
       </c>
       <c r="F20" s="42">
         <v>51</v>
@@ -2963,46 +2958,46 @@
       <c r="G20" s="68"/>
       <c r="O20" s="68"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16">
       <c r="B21" s="79" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="83" t="s">
+        <v>199</v>
+      </c>
+      <c r="E21" s="41" t="s">
         <v>200</v>
-      </c>
-      <c r="E21" s="41" t="s">
-        <v>201</v>
       </c>
       <c r="F21" s="72">
         <v>52</v>
       </c>
-      <c r="H21" s="110" t="s">
-        <v>172</v>
-      </c>
-      <c r="I21" s="111"/>
-      <c r="J21" s="111"/>
-      <c r="K21" s="111"/>
-      <c r="L21" s="111"/>
-      <c r="M21" s="112"/>
+      <c r="H21" s="107" t="s">
+        <v>171</v>
+      </c>
+      <c r="I21" s="108"/>
+      <c r="J21" s="108"/>
+      <c r="K21" s="108"/>
+      <c r="L21" s="108"/>
+      <c r="M21" s="109"/>
       <c r="O21" s="68"/>
     </row>
-    <row r="22" spans="2:16" ht="45" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="42">
       <c r="B22" s="77" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="59" t="s">
+        <v>201</v>
+      </c>
+      <c r="E22" s="41" t="s">
         <v>202</v>
-      </c>
-      <c r="E22" s="41" t="s">
-        <v>203</v>
       </c>
       <c r="F22" s="73">
         <v>53</v>
       </c>
-      <c r="H22" s="101" t="s">
-        <v>312</v>
+      <c r="H22" s="112" t="s">
+        <v>311</v>
       </c>
       <c r="I22" s="82" t="s">
         <v>156</v>
@@ -3017,16 +3012,16 @@
         <v>159</v>
       </c>
       <c r="M22" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O22" s="68"/>
     </row>
-    <row r="23" spans="2:16" ht="45" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="42">
       <c r="B23" s="79" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C23" s="8"/>
-      <c r="H23" s="102"/>
+      <c r="H23" s="113"/>
       <c r="I23" s="82" t="s">
         <v>160</v>
       </c>
@@ -3040,69 +3035,69 @@
         <v>159</v>
       </c>
       <c r="M23" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O23" s="68"/>
     </row>
-    <row r="24" spans="2:16" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="42">
       <c r="B24" s="79" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C24" s="8"/>
       <c r="H24" s="90" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I24" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="J24" s="39" t="s">
         <v>220</v>
       </c>
-      <c r="J24" s="39" t="s">
+      <c r="K24" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="K24" s="38" t="s">
+      <c r="L24" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="L24" s="38" t="s">
-        <v>223</v>
-      </c>
       <c r="M24" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O24" s="68"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16">
       <c r="B25" s="79" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D25" s="43"/>
       <c r="E25" s="7"/>
       <c r="F25" s="45"/>
       <c r="O25" s="68"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16">
       <c r="B26" s="79" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D26" s="43"/>
       <c r="E26" s="7"/>
       <c r="F26" s="45"/>
-      <c r="H26" s="110" t="s">
-        <v>173</v>
-      </c>
-      <c r="I26" s="111"/>
-      <c r="J26" s="111"/>
-      <c r="K26" s="111"/>
-      <c r="L26" s="111"/>
-      <c r="M26" s="112"/>
+      <c r="H26" s="107" t="s">
+        <v>172</v>
+      </c>
+      <c r="I26" s="108"/>
+      <c r="J26" s="108"/>
+      <c r="K26" s="108"/>
+      <c r="L26" s="108"/>
+      <c r="M26" s="109"/>
       <c r="O26" s="68"/>
     </row>
-    <row r="27" spans="2:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="28">
       <c r="B27" s="46" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="45"/>
-      <c r="H27" s="103" t="s">
-        <v>250</v>
+      <c r="H27" s="114" t="s">
+        <v>249</v>
       </c>
       <c r="I27" s="82" t="s">
         <v>163</v>
@@ -3117,18 +3112,18 @@
         <v>42</v>
       </c>
       <c r="M27" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O27" s="68"/>
     </row>
-    <row r="28" spans="2:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="28">
       <c r="B28" s="79" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="62"/>
       <c r="F28" s="64"/>
-      <c r="H28" s="104"/>
+      <c r="H28" s="115"/>
       <c r="I28" s="82" t="s">
         <v>169</v>
       </c>
@@ -3142,15 +3137,15 @@
         <v>43</v>
       </c>
       <c r="M28" s="72" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="O28" s="68"/>
     </row>
-    <row r="29" spans="2:16" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="28">
       <c r="D29" s="63"/>
       <c r="E29" s="62"/>
       <c r="F29" s="64"/>
-      <c r="H29" s="105"/>
+      <c r="H29" s="116"/>
       <c r="I29" s="83" t="s">
         <v>44</v>
       </c>
@@ -3158,66 +3153,66 @@
         <v>40</v>
       </c>
       <c r="K29" s="82" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="L29" s="82" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M29" s="72" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" s="61" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" s="61" customFormat="1" ht="28">
       <c r="B30" s="2"/>
       <c r="D30" s="43"/>
       <c r="E30" s="7"/>
       <c r="F30" s="45"/>
-      <c r="H30" s="106" t="s">
-        <v>312</v>
+      <c r="H30" s="117" t="s">
+        <v>311</v>
       </c>
       <c r="I30" s="83" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J30" s="83" t="s">
         <v>139</v>
       </c>
       <c r="K30" s="82" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L30" s="82" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M30" s="82" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" s="61" customFormat="1" ht="30" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" s="61" customFormat="1" ht="28">
       <c r="D31" s="43"/>
       <c r="E31" s="7"/>
       <c r="F31" s="45"/>
-      <c r="H31" s="107"/>
+      <c r="H31" s="118"/>
       <c r="I31" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J31" s="83" t="s">
         <v>140</v>
       </c>
       <c r="K31" s="82" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="L31" s="82" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="M31" s="82" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" ht="60" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="56">
       <c r="D32" s="43"/>
       <c r="E32" s="7"/>
       <c r="F32" s="45"/>
       <c r="H32" s="96" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="I32" s="83" t="s">
         <v>145</v>
@@ -3226,242 +3221,247 @@
         <v>146</v>
       </c>
       <c r="K32" s="82" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L32" s="82" t="s">
         <v>147</v>
       </c>
       <c r="M32" s="72" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="33" spans="4:14" ht="30" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" ht="28">
       <c r="H33" s="96" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I33" s="83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J33" s="83" t="s">
         <v>146</v>
       </c>
       <c r="K33" s="82" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L33" s="82" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M33" s="82" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="N33" s="23"/>
     </row>
-    <row r="34" spans="4:14" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:14" ht="28">
       <c r="D34" s="43"/>
       <c r="E34" s="7"/>
       <c r="F34" s="45"/>
       <c r="H34" s="74" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I34" s="39" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J34" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="K34" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="K34" s="38" t="s">
+      <c r="L34" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="L34" s="38" t="s">
-        <v>226</v>
-      </c>
       <c r="M34" s="72" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="35" spans="4:14" ht="30" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" ht="28">
       <c r="D35" s="43"/>
       <c r="E35" s="7"/>
       <c r="F35" s="45"/>
-      <c r="H35" s="108" t="s">
-        <v>287</v>
+      <c r="H35" s="119" t="s">
+        <v>286</v>
       </c>
       <c r="I35" s="83" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J35" s="81" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K35" s="81" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L35" s="85" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M35" s="82" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="36" spans="4:14" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" ht="30" customHeight="1">
       <c r="D36" s="47"/>
       <c r="E36" s="6"/>
       <c r="F36" s="48"/>
-      <c r="H36" s="109"/>
+      <c r="H36" s="120"/>
       <c r="I36" s="83" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J36" s="81" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K36" s="81" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L36" s="85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M36" s="82" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="37" spans="4:14" ht="30" x14ac:dyDescent="0.2">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" ht="28">
       <c r="D37" s="47"/>
       <c r="E37" s="7"/>
       <c r="F37" s="48"/>
       <c r="H37" s="74" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I37" s="39" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J37" s="39" t="s">
+        <v>226</v>
+      </c>
+      <c r="K37" s="38" t="s">
         <v>227</v>
       </c>
-      <c r="K37" s="38" t="s">
+      <c r="L37" s="38" t="s">
         <v>228</v>
       </c>
-      <c r="L37" s="38" t="s">
-        <v>229</v>
-      </c>
       <c r="M37" s="72" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="38" spans="4:14" ht="30" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" ht="28">
       <c r="H38" s="74">
         <v>53</v>
       </c>
       <c r="I38" s="39" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J38" s="39" t="s">
+        <v>243</v>
+      </c>
+      <c r="K38" s="82" t="s">
+        <v>243</v>
+      </c>
+      <c r="L38" s="86" t="s">
         <v>244</v>
       </c>
-      <c r="K38" s="82" t="s">
-        <v>244</v>
-      </c>
-      <c r="L38" s="86" t="s">
-        <v>245</v>
-      </c>
       <c r="M38" s="72" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="44" spans="4:14" x14ac:dyDescent="0.2">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14">
       <c r="D44" s="49"/>
       <c r="E44" s="49"/>
       <c r="F44" s="49"/>
     </row>
-    <row r="45" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:14">
       <c r="D45" s="50"/>
       <c r="E45" s="51"/>
       <c r="F45" s="52"/>
     </row>
-    <row r="46" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:14">
       <c r="D46" s="50"/>
       <c r="E46" s="51"/>
       <c r="F46" s="52"/>
     </row>
-    <row r="47" spans="4:14" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:14" ht="32.25" customHeight="1">
       <c r="D47" s="50"/>
       <c r="E47" s="51"/>
       <c r="F47" s="52"/>
     </row>
-    <row r="48" spans="4:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="4:14">
       <c r="D48" s="50"/>
       <c r="E48" s="53"/>
       <c r="F48" s="52"/>
     </row>
-    <row r="49" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="4:6">
       <c r="D49" s="50"/>
       <c r="E49" s="51"/>
       <c r="F49" s="52"/>
     </row>
-    <row r="55" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="4:6">
       <c r="D55" s="54"/>
     </row>
-    <row r="56" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="4:6">
       <c r="D56" s="54"/>
     </row>
-    <row r="59" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="4:6">
       <c r="D59" s="54"/>
     </row>
-    <row r="60" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="4:6">
       <c r="D60" s="54"/>
     </row>
-    <row r="61" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="4:6">
       <c r="D61" s="54"/>
     </row>
-    <row r="72" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="4:6">
       <c r="D72" s="55"/>
       <c r="E72" s="55"/>
       <c r="F72" s="55"/>
     </row>
-    <row r="73" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="4:6">
       <c r="D73" s="56"/>
       <c r="E73" s="57"/>
       <c r="F73" s="58"/>
     </row>
-    <row r="74" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="4:6">
       <c r="D74" s="56"/>
       <c r="E74" s="57"/>
       <c r="F74" s="58"/>
     </row>
-    <row r="75" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="4:6">
       <c r="D75" s="56"/>
       <c r="E75" s="57"/>
       <c r="F75" s="58"/>
     </row>
-    <row r="76" spans="4:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="4:6">
       <c r="D76" s="56"/>
       <c r="E76" s="57"/>
       <c r="F76" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="H6:M6"/>
+    <mergeCell ref="H26:M26"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="H4:M4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="D18:F18"/>
     <mergeCell ref="H11:M11"/>
     <mergeCell ref="H12:H13"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="H21:M21"/>
     <mergeCell ref="H17:M17"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="H4:M4"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="H6:M6"/>
-    <mergeCell ref="H26:M26"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
   <ignoredErrors>
     <ignoredError sqref="H9" numberStoredAsText="1"/>
   </ignoredErrors>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3471,14 +3471,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="105.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
         <v>141</v>
       </c>
@@ -3489,121 +3489,121 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" s="60" customFormat="1">
       <c r="A2" s="67">
         <v>42348</v>
       </c>
       <c r="B2" s="93"/>
       <c r="C2" s="99" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" s="60" customFormat="1">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="60" customFormat="1">
       <c r="A4" s="67">
         <v>42347</v>
       </c>
       <c r="B4" s="93"/>
       <c r="C4" s="99" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="60" customFormat="1">
       <c r="A5" s="67"/>
       <c r="B5" s="93"/>
       <c r="C5" s="99" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="60" customFormat="1">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" s="66" customFormat="1">
       <c r="A7" s="67">
         <v>42340</v>
       </c>
       <c r="B7" s="69"/>
       <c r="C7" s="65" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="66" customFormat="1">
       <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:3" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" s="70" customFormat="1">
       <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" s="66" customFormat="1">
       <c r="A10" s="3"/>
       <c r="B10" s="1"/>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" s="66" customFormat="1">
       <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11"/>
     </row>
-    <row r="12" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" s="66" customFormat="1">
       <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12"/>
     </row>
-    <row r="13" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" s="66" customFormat="1">
       <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13"/>
     </row>
-    <row r="14" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" s="66" customFormat="1">
       <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14"/>
     </row>
-    <row r="15" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" s="66" customFormat="1">
       <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15"/>
     </row>
-    <row r="16" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" s="66" customFormat="1">
       <c r="A16" s="3"/>
       <c r="B16" s="1"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="66" customFormat="1">
       <c r="A17" s="3"/>
       <c r="B17" s="1"/>
       <c r="C17"/>
     </row>
-    <row r="18" spans="1:3" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="70" customFormat="1">
       <c r="A18" s="3"/>
       <c r="B18" s="1"/>
       <c r="C18"/>
     </row>
-    <row r="19" spans="1:3" s="68" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="68" customFormat="1">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19"/>
     </row>
-    <row r="20" spans="1:3" s="70" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="70" customFormat="1">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20"/>
     </row>
-    <row r="21" spans="1:3" s="66" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="66" customFormat="1">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21"/>
     </row>
-    <row r="22" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="60" customFormat="1">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22"/>
@@ -3611,7 +3611,12 @@
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -3621,720 +3626,725 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="105.5" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1">
       <c r="A3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1">
       <c r="A4" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1">
       <c r="A5" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1">
       <c r="A6" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1">
       <c r="A13" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1">
       <c r="A14" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1">
       <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1">
       <c r="A16" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1">
       <c r="A27" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1">
       <c r="A28" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1">
       <c r="A29" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1">
       <c r="A31" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1">
       <c r="A32" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1">
       <c r="A33" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1">
       <c r="A34" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1">
       <c r="A35" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1">
       <c r="A36" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1">
       <c r="A37" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1">
       <c r="A38" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1">
       <c r="A39" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1">
       <c r="A40" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1">
       <c r="A41" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1">
       <c r="A42" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1">
       <c r="A43" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1">
       <c r="A44" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1">
       <c r="A45" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1">
       <c r="A46" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1">
       <c r="A47" s="87" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
       <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1">
       <c r="A49" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1">
       <c r="A50" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1">
       <c r="A51" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1">
       <c r="A52" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1">
       <c r="A53" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1">
       <c r="A54" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1">
       <c r="A56" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1">
       <c r="A57" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1">
       <c r="A58" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1">
       <c r="A59" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1">
       <c r="A60" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1">
       <c r="A61" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1">
       <c r="A62" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1">
       <c r="A63" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1">
       <c r="A64" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1">
       <c r="A65" s="2" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1">
       <c r="A66" s="2" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1">
       <c r="A67" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1">
       <c r="A68" s="88" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
       <c r="A69" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:1">
       <c r="A70" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:1">
       <c r="A71" s="2" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:1">
       <c r="A72" s="2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:1">
       <c r="A73" s="2" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:1">
       <c r="A74" s="2" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:1">
       <c r="A75" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:1">
       <c r="A77" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:1">
       <c r="A78" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:1">
       <c r="A79" s="2" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:1">
       <c r="A80" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:1">
       <c r="A81" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:1">
       <c r="A82" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:1">
       <c r="A83" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:1">
       <c r="A84" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:1">
       <c r="A85" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:1">
       <c r="A86" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:1">
       <c r="A87" s="2" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:1">
       <c r="A88" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:1">
       <c r="A89" s="89" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
       <c r="A90" s="2" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:1">
       <c r="A91" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:1">
       <c r="A92" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:1">
       <c r="A93" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:1">
       <c r="A94" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:1">
       <c r="A95" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:1">
       <c r="A96" s="2" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:1">
       <c r="A98" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:1">
       <c r="A99" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:1">
       <c r="A100" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:1">
       <c r="A101" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:1">
       <c r="A102" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:1" s="60" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:1" s="60" customFormat="1">
       <c r="A103" s="89" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" s="60" customFormat="1">
+      <c r="A104" s="89" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="104" spans="1:1" s="60" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="89" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:1">
       <c r="A106" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:1">
       <c r="A107" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:1">
       <c r="A108" s="89" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
       <c r="A109" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:1">
       <c r="A110" s="80" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
       <c r="A111" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:1">
       <c r="A112" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:1">
       <c r="A113" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:1">
       <c r="A114" s="80" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="80" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="80" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:1">
       <c r="A116" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:1">
       <c r="A117" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:1">
       <c r="A118" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:1">
       <c r="A119" s="89" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="89" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="89" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:1">
       <c r="A122" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:1">
       <c r="A123" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:1">
       <c r="A124" s="89" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
       <c r="A125" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:1">
       <c r="A126" s="80" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
       <c r="A127" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:1">
       <c r="A128" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:1">
       <c r="A129" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1">
       <c r="A130" s="80" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="80" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A131" s="80" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:1">
       <c r="A132" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:1">
       <c r="A133" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:1">
       <c r="A134" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:1">
       <c r="A135" s="89" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="89" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A136" s="89" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:1">
       <c r="A138" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:1">
       <c r="A139" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:1">
       <c r="A140" s="89" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
       <c r="A141" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:1">
       <c r="A142" s="80" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
       <c r="A143" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:1">
       <c r="A144" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:1">
       <c r="A145" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:1">
       <c r="A146" s="80" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="80" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A147" s="80" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:1">
       <c r="A148" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:1">
       <c r="A149" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:1">
       <c r="A150" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:1">
       <c r="A151" s="89" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="89" t="s">
         <v>267</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="89" t="s">
-        <v>268</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -4344,91 +4354,91 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="43.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>175</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>176</v>
       </c>
       <c r="B2" s="1">
         <v>203</v>
       </c>
       <c r="C2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B3" s="1">
         <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B4" s="1">
         <v>209</v>
       </c>
       <c r="C4" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B5" s="1">
         <v>207</v>
       </c>
       <c r="C5" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="60" customFormat="1">
       <c r="A6" s="60" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="1">
         <v>210</v>
       </c>
       <c r="C6" s="60" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B7" s="1">
         <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>33</v>
       </c>
@@ -4436,10 +4446,10 @@
         <v>112</v>
       </c>
       <c r="C8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -4447,49 +4457,54 @@
         <v>113</v>
       </c>
       <c r="C9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="60" customFormat="1" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="60" customFormat="1">
       <c r="A10" s="60" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B11" s="1">
         <v>311</v>
       </c>
       <c r="C11" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B12" s="1">
         <v>312</v>
       </c>
       <c r="C12" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="60" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B13" s="1">
         <v>313</v>
       </c>
       <c r="C13" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>